<commit_message>
extended gemini training set
</commit_message>
<xml_diff>
--- a/clean/gemini_training_set.xlsx
+++ b/clean/gemini_training_set.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B512"/>
+  <dimension ref="A1:B495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17479,648 +17479,6 @@
         </is>
       </c>
     </row>
-    <row r="496">
-      <c r="A496" t="inlineStr">
-        <is>
-          <t># Friche de la Belle de Mai
-Salles de spectacle, expositions, terrains de foot, basket, skate…
-#### Adresse
-41 Rue Jobin, 13003 Marseille
-#### Horaires d'ouverture
--
-##### Jrs. ouvrables (Lun - Ven)
-- 08:30 - 00:00
-##### samedi
-- 08:30 - 00:00
-##### dimanche
-- 08:30 - 22:00
-#### Contacts
--
-[Site](http://www.lafriche.org/fr/) -
-[+33495049595](tel:+33495049595)
-#### Proposer une modification
--
-[Écrire à QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Merci de modifier les infos de ce lieu&amp;body=Friche de la Belle de Mai (https://qx1.org/lieu/friche-de-la-belle-de-mai/) )</t>
-        </is>
-      </c>
-      <c r="B496" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_cultural_and_social_events_marseille", "info": "I am looking for a place in Marseille to attend cultural events, concerts, exhibitions, or social gatherings."}, {"id": "need_sports_facilities_marseille", "info": "I need to find sports facilities in Marseille, such as a football stadium, basketball court, or skate park."}], "Summary": {"country": "FR", "description": "La Friche de la Belle de Mai is a large cultural and social center in Marseille, France. It offers various spaces and facilities, including performance venues, exhibitions, sports fields, and a library.", "id": "friche_de_la_belle_de_mai_marseille", "type": "directory", "cities": ["Marseille"]}, "Contact": [{"id": "contact_la_friche_marseille", "phone": "+33495049595", "contact_page": "http://www.lafriche.org/fr/", "city": "Marseille"}], "Organization": [{"id": "la_friche_belle_de_mai", "info": "La Friche de la Belle de Mai is a cultural and social center in Marseille, offering various activities.", "cities": ["Marseille"], "contacts": ["contact_la_friche_marseille"]}], "Provision": [{"contexts": ["need_cultural_and_social_events_marseille"], "id": "cultural_and_social_events", "info": "Providing access to spaces for performances, exhibitions, and events.", "organizations": ["la_friche_belle_de_mai"]}, {"contexts": ["need_sports_facilities_marseille"], "id": "sports_facilities_access", "info": "Providing access to sports fields and equipment.", "organizations": ["la_friche_belle_de_mai"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="497">
-      <c r="A497" t="inlineStr">
-        <is>
-          <t># Corhesan (mobile health mediation team)
-CORHESAN is a mobile team of health mediators who help residents of the 1st, 2nd and 3rd arrondissements with :
-- Cancer screening: breast, cervix, colon
-- Finding an appointment for a mammogram or smear test
-- Picking up your colorectal screening kit
-- Vaccination catch-up: DTP, HPV, Hep B, flu, Covid, etc.
-- Access to healthcare rights
-- Access to health rights
-- Finding a GP
-Instagram: https://www.instagram.com/corhesan/
-Facebook: https://www.facebook.com/Corhesan/
-#### Address
-Hôpital Européen Marseille, Rue Désirée Clary, Marseille, France
-#### Further directions
-Parvis de l'Hôpital Européen, à droite des urgences
-#### Contacts
--
-[Website](https://www.hopital-europeen.fr/corhesan) -
-[corhesan@gmail.com](mailto:corhesan@gmail.com) -
-[+33413427805](tel:+33413427805)
-#### Suggest an edit
--
-[Write to QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Please, edit this place info&amp;body=Corhesan (mobile health mediation team) (https://qx1.org/en/place/corhesan-mobile-health-mediation-team/) )</t>
-        </is>
-      </c>
-      <c r="B497" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_cancer_screening", "info": "I need to get screened for cancer (breast, cervix, or colon)."}, {"id": "need_mammogram_or_smear_test_appointment", "info": "I need to schedule an appointment for a mammogram or smear test."}, {"id": "need_colorectal_screening_kit", "info": "I need to pick up a colorectal screening kit."}, {"id": "need_vaccination_catch_up", "info": "I need to get caught up on vaccinations (DTP, HPV, Hep B, flu, Covid, etc.)."}, {"id": "need_to_access_healthcare_rights", "info": "I need to know more about my rights to healthcare in France."}, {"id": "need_to_find_gp", "info": "I need to find a general practitioner (GP) in France."}, {"id": "need_to_access_hospital_services", "info": "I need to access hospital services."}], "Summary": {"country": "FR", "description": "CORHESAN is a mobile team of health mediators in Marseille, France, offering cancer screenings, vaccination catch-up, and assistance with accessing healthcare rights.", "id": "corhesan_marseille", "type": "directory", "cities": ["Marseille"]}, "Contact": [{"id": "contact_corhesan_email_marseille", "email": "corhesan@gmail.com", "city": "Marseille"}, {"id": "contact_corhesan_email_marseille", "city": "Marseille", "address": "Hôpital Européen Marseille, Rue Désirée Clary, Marseille, France", "phone": "+33413427805", "email": "corhesan@gmail.com"}], "Organization": [{"id": "corhesan", "info": "CORHESAN is a mobile team of health mediators that helps residents of the 1st, 2nd, and 3rd arrondissements in Marseille access healthcare.", "cities": ["Marseille"], "contacts": ["contact_corhesan_email_marseille"]}, {"id": "hopital_europeen_marseille", "info": "Hôpital Européen Marseille is a hospital.", "cities": ["Marseille"]}], "Provision": [{"contexts": ["need_cancer_screening", "need_mammogram_or_smear_test_appointment", "need_colorectal_screening_kit"], "id": "cancer_screening_and_support", "info": "Providing cancer screening services, scheduling mammograms and smear tests, and helping individuals collect colorectal screening kits.", "organizations": ["corhesan"]}, {"contexts": ["need_vaccination_catch_up"], "id": "vaccination_catch_up_services", "info": "Offering vaccination catch-up services.", "organizations": ["corhesan"]}, {"contexts": ["need_to_access_healthcare_rights"], "id": "healthcare_rights_information", "info": "Providing information about healthcare rights.", "organizations": ["corhesan"]}, {"contexts": ["need_to_find_gp"], "id": "general_practitioner_referral", "info": "Helping individuals find a general practitioner (GP).", "organizations": ["corhesan"]}, {"contexts": ["need_to_access_hospital_services"], "id": "hospital_services", "info": "Providing hospital services.", "organizations": ["hopital_europeen_marseille"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="498">
-      <c r="A498" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Le séjour pour motif de santé (PASS Rimbaud)
-Deux jours après, lors d’un deuxième rendez-vous en Préfecture, j’ai pu parler de mes conditions de santé ; on m’a donné un certificat médical pour l’OFII. Je devais donc aller voir un médecin, faire les analyses nécessaires pour qu’il constate mes problèmes de santé et remplisse ce papier.
-Je me suis rendu à l’Hôpital de la Timone, au service PASS Rimbaud, et j’ai postérieurement envoyé le certificat à l’OFII, par recommandée.
-Retourné à la Préfecture, j’ai eu un permis de séjour d’un mois (récépissé), m’autorisant à rester sur le territoire français pendant que mon dossier est étudié.
-[Officefrançaisdel’Immigrationetl’Intégration(OFII)](https://qx1.org/lieu/office-francais-de-limmigration-et-lintegration-ofii/)
-L’accueil des demandeurs d’asile L’OFII est responsable du Premier accueil des demandeurs d’asile et gère le dispositif national d’accueil L’OFII pilote et finance les structures de premier accueil des demandeurs d’asile (SPADA) dans le cadre d’un marché public passé avec des opérateurs extérieurs et ouvre les conditions matérielles d’accueil (CMA) aux demandeurs d’asile après leur passage en guichet unique pour demandeurs d’asile (GUDA) [...]
-[PASSAdultes(H.Nord)](https://qx1.org/lieu/pass-adultes-hopital-nord/)
-Permanence d’Accès aux Soins de Santé pour personnes en situation de précarité (n'ayant pas de CMU ou AME) : infirmiers, médécin, ouverture des droits...
-[Préfecture(Étrangers–SiteSaintSébastien)](https://qx1.org/lieu/prefecture-etrangers-site-saint-sebastien/)
-Ce site regroupe les services de délivrance des titres: la direction des étrangers et de la nationalité la direction de la réglementation et des libertés publiques (certificats d’immatriculations, permis de conduire, cartes nationales d’identité, passeports)
-</t>
-        </is>
-      </c>
-      <c r="B498" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_to_access_healthcare_services", "info": "I need access to healthcare services, such as medical consultations or examinations."}, {"id": "need_medical_certification", "info": "I need a medical certificate to support my administrative procedures."}, {"id": "need_to_understand_french_immigration_system", "info": "I need information about the French immigration system."}], "Summary": {"country": "FR", "description": "This guide recounts the experience of a migrant in Marseille, France, seeking to obtain a residence permit based on their health condition. It highlights the process of receiving a medical certificate, submitting it to the OFII, and obtaining a temporary residence permit while the application is being processed.", "id": "residence_permit_health_reasons_marseille", "type": "experience", "cities": ["Marseille"]}, "Organization": [{"id": "pass_rimbaud", "info": "PASS Rimbaud is a healthcare access point in Marseille.", "cities": ["Marseille"]}, {"id": "la_timone_hospital", "info": "A hospital in Marseille.", "cities": ["Marseille"]}, {"id": "ofii", "info": "The Office Français de l'Immigration et de l'Intégration (OFII) is the French Office for Immigration and Integration, which provides support to asylum seekers."}], "Provision": [{"contexts": ["need_medical_certification"], "id": "medical_certification_services", "info": "Providing medical certificates that can support administrative procedures.", "organizations": ["pass_rimbaud"]}, {"contexts": ["need_to_access_healthcare_services"], "id": "hospital_services", "info": "Providing medical evaluations and treatment.", "organizations": ["la_timone_hospital"]}, {"contexts": ["need_to_understand_french_immigration_system"], "id": "immigration_system_information_and_guidance", "info": "Providing information and guidance on immigration processes.", "organizations": ["ofii"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="499">
-      <c r="A499" t="inlineStr">
-        <is>
-          <t># Être accompagné dans votre projet professionnel et vos démarches
-C'est quoi ?
-Un ** parcours entièrement personnalisé** qui peut durer de 6 à 18 mois
-**et**
-**pour les jeunes âgés de 16 à 25 ans**
-**aux personnes moins de 30 ans en situation de handicap.**Cet accompagnement intensif aide à :
-- faire les démarches de la vie quotidienne
-- construire son projet professionnel
-- trouver une formation ou un travail.
-L'objectif est d'être le plus autonome possible dans sa vie quotidienne et professionnelle.
-Il est possible de recevoir une aide financière tous les mois sous conditions.
-- avoir entre 16 et 25 ans, ou moins de 30 ans en situation de handicap bénéficiant d’une reconnaissance de la qualité de travailleur handicapé (RQTH),
-- ne pas être en formation, ni en études, ni en activité professionnelle.
-Pourquoi c'est intéressant ?
-La Mission Locale vous aide à :
-- faire les démarches administratives (carte de séjour, papiers d’identité...)
-- ouvrir vos droits à la santé et au logement (demande de logement social, attestation de sécurité sociale…)
-Vous devez participer à différentes activités pour rencontrer des professionnels et développer vos compétences, par exemple :
-- atelier d'orientation pour vous aider à trouver un métier/une formation
-- atelier pour apprendre le français
-- atelier mathématiques
-- atelier pour se préparer à l'entretien d'embauche
-- atelier sur la citoyenneté et le droit des étrangers
-- visite et stage en entreprise...
-Si vous respectez l'engagement d'être présent à toutes les activités (entre 15 heures et 20 heures par semaine) et d'assister aux rendez-vous hebdomadaires, vous pouvez en fonction de votre situation recevoir une aide financière :
-- 528 € par mois pour les personnes majeures
-- 211,20 € pour les personnes mineures.
-Comment faire ?
-: 03 82 82 85 15**Par téléphone****Par mail**[: contact.thionville@mlnm.fr](https://www.mlnm.fr/nous-contacter/prise-de-rendez-vous-thionville/): Siège social - Mission Locale du Nord Mosellan - Locaux de l'AFPA, Bâtiment, 12 Rte d'Illange, 57970 Yutz**Directement sur place**</t>
-        </is>
-      </c>
-      <c r="B499" t="inlineStr">
-        <is>
-          <t>{"Contact": [{"id": "contact_mission_locale_thionville", "phone": "03 82 82 85 15", "email": "contact.thionville@mlnm.fr", "city": "Thionville"}], "Organization": [{"id": "mission_locale_nord_mosellan", "info": "Mission Locale du Nord Mosellan provides intensive support to young people and those with disabilities.", "contacts": ["contact_mission_locale_thionville"], "cities": ["Thionville", "Yutz"], "website": "https://www.mlnm.fr/"}], "Summary": {"country": "FR", "description": "Mission Locale du Nord Mosellan provides an intensive, personalized support program for young people (16-25 years old) and individuals under 30 with disabilities in the Thionville region of France. The program offers assistance with daily tasks, career development, training, and job searching, and may include financial aid.", "id": "mission_locale_nord_mosellan_support", "type": "guide", "cities": ["Thionville", "Yutz"]}, "Context": [{"id": "need_career_support_thionville", "info": "I am a young person (16-25 years old) or an individual under 30 with a disability in the Thionville region, France, and need help with my career development and daily life."}, {"id": "need_financial_aid_thionville", "info": "I am a young person (16-25 years old) or an individual under 30 with a disability in the Thionville region, France, and need financial aid."}], "Provision": [{"contexts": ["need_career_support_thionville", "need_financial_aid_thionville"], "id": "personalized_career_support", "info": "Providing personalized support for young people and those with disabilities to help with daily life, career development, training, and job searching, and offering financial aid under certain conditions.", "organizations": ["mission_locale_nord_mosellan"]}], "Task": [{"contexts": ["need_career_support_thionville", "need_financial_aid_thionville"], "id": "contact_mission_locale_thionville", "info": "Contacting Mission Locale du Nord Mosellan for support.", "contacts": "contact_mission_locale_thionville", "provisions": ["personalized_career_support"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="500">
-      <c r="A500" t="inlineStr">
-        <is>
-          <t># Marché de Noailles (Noailles market)
-Market selling fruit, vegetables, meat, fish, household products and meals at reasonable prices.
-The district is also home to a number of community associations.
-#### Address
-Noailles, Marseille, France
-#### Suggest an edit
--
-[Write to QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Please, edit this place info&amp;body=Marché de Noailles (Noailles market) (https://qx1.org/en/place/marche-de-noailles-noailles-market/) )</t>
-        </is>
-      </c>
-      <c r="B500" t="inlineStr">
-        <is>
-          <t>{"Summary": {"country": "FR", "description": "A marketplace in Marseille, France offering a variety of goods and services.", "id": "marche_de_noailles", "type": "place", "cities": ["Marseille"]}, "Context": [{"id": "need_to_shop_noailles", "info": "I need to shop for food, household items, or prepared meals."}], "Organization": [{"id": "noailles_community_associations", "info": "Community associations located in the Noailles district of Marseille.", "cities": ["Marseille"]}], "Provision": [{"contexts": ["need_to_shop_noailles"], "id": "market_goods_and_services", "info": "Selling fruit, vegetables, meat, fish, household products, and ready-to-eat meals at reasonable prices.", "organizations": ["noailles_community_associations"]}], "Task": [{"contexts": ["need_to_shop_noailles"], "id": "shop_at_noailles_market", "info": "Shopping at the Noailles Market.", "provisions": ["market_goods_and_services"]}], "Contact": [{"id": "contact_noailles_community_associations_marseille", "address": "Noailles, Marseille, France", "city": "Marseille"}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="501">
-      <c r="A501" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Trouver un travail dans le secteur de l'électroménager
-C'est quoi ?
-La structure ENVIE est spécialisée dans la récupération, la réparation et le traitement des déchets électroménagers.
-Elle embauche et forme des personnes pour différents postes : réparateur d'appareils électroménagers, chauffeur livreur, magasinier, conducteur de poids lourd, vendeur, trieurs de pièces détachées...
-Les produits sont ensuite vendus dans un magasin à Gerzat (machines à laver, fours, réfrigérateurs, fours micro-ondes...).
-Pourquoi c'est intéressant ?
-Vous êtes accompagné par des professionnels qui vous aident à savoir quel métier est le plus adapté, en fonction de vos compétences et des possibilités.
-Le chantier d'insertion aide à trouver un travail fixe, à faire partie d'une entreprise, à rencontrer des collègues...
-Vous apprenez un métier avec une formation spéciale, des conseils, des techniques professionnelles.
-En fonction de vos capacités, il est aussi possible de travailler à différents postes.
-Comment faire ?
-Utilisez votre compte Pôle Emploi pour vous inscrire sur la [plateforme de l'inclusion](https://emplois.inclusion.beta.gouv.fr/accounts/login/?next=/apply/5490/start), ou demandez à votre conseiller, à votre assistant social, à la mission locale de se connecter pour vous orienter.
-Les métiers proposés par Envie M.O. sont ici : [https://emplois.inclusion.beta.gouv.fr/](https://emplois.inclusion.beta.gouv.fr/company/5490/card?back_url=/search/employers/results%3Fcity%3Dclermont-ferrand-63%26city_name%3D%26distance%3D25%26kinds%3DEI)
-- Par mail :
-[contact-enviemo@envie.org](mailto:contact-enviemo@envie.org) - Par téléphone : 04 73 25 06 98
-## Addresses
-### ENVIE MO
-6 Rue Pierre et Marie Curie, 63360 Gerzat, France
-</t>
-        </is>
-      </c>
-      <c r="B501" t="inlineStr">
-        <is>
-          <t>{"Contact": [{"id": "contact_envie_mo_gerzat", "email": "contact-enviemo@envie.org", "phone": "04 73 25 06 98", "city": "Gerzat"}, {"id": "platform_inclusion_contact", "contact_page": "https://emplois.inclusion.beta.gouv.fr/accounts/login/?next=/apply/5490/start"}, {"id": "contact_envie_mo_gerzat", "address": "6 Rue Pierre et Marie Curie, 63360 Gerzat, France", "city": "Gerzat", "phone": "04 73 25 06 98", "email": "contact-enviemo@envie.org"}], "Context": [{"id": "need_job_in_appliance_repair", "info": "I am looking for a job in the appliance repair sector."}, {"id": "need_job_training_appliance_repair", "info": "I need training and experience in appliance repair to find a job."}, {"id": "need_assistance_finding_job_appliance_repair", "info": "I need help finding a job in appliance repair."}], "Summary": {"country": "FR", "description": "ENVIE MO is a social enterprise that provides job training and employment opportunities in the appliance repair sector.", "id": "job_appliance_repair_envie_mo", "type": "guide", "cities": ["Gerzat"]}, "Organization": [{"id": "envie_mo", "info": "ENVIE MO is a social enterprise specializing in appliance repair and recycling.", "contacts": ["contact_envie_mo_gerzat"], "cities": ["Gerzat"]}, {"id": "pole_emploi", "info": "Pôle Emploi is the French employment agency.", "cities": ["Gerzat"]}, {"id": "mission_locale", "info": "Mission Locale is a local organization that provides support to young people seeking employment.", "cities": ["Gerzat"]}], "Provision": [{"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "appliance_repair_job_training", "info": "Providing job training and employment opportunities in the appliance repair sector.", "organizations": ["envie_mo"]}, {"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "job_search_assistance_pole_emploi", "info": "Providing job search assistance and guidance.", "organizations": ["pole_emploi"]}, {"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "job_search_assistance_mission_locale", "info": "Providing job search assistance and guidance for young people.", "organizations": ["mission_locale"]}], "Task": [{"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "register_on_platform_inclusion", "info": "Register on the platform de l'inclusion.", "contacts": "platform_inclusion_contact", "provisions": ["appliance_repair_job_training"]}, {"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "contact_pole_emploi", "info": "Contact Pôle Emploi for job search assistance.", "provisions": ["job_search_assistance_pole_emploi"]}, {"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "contact_mission_locale", "info": "Contact Mission Locale for job search assistance.", "provisions": ["job_search_assistance_mission_locale"]}, {"contexts": ["need_job_in_appliance_repair", "need_job_training_appliance_repair", "need_assistance_finding_job_appliance_repair"], "id": "contact_envie_mo_directly", "info": "Contact ENVIE MO directly for job information and opportunities.", "contacts": "contact_envie_mo", "provisions": ["appliance_repair_job_training"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="502">
-      <c r="A502" t="inlineStr">
-        <is>
-          <t># CCAS (Community Social Action Center) – Center Agency
-The CCAS center covers the 1st, 2nd, 3rd and 7th arrondissement.
-The CCAS, Community Social Action Center, provides help and support to people in difficulty: families, the elderly, the disabled, the homeless or those in precarious situations…
-Their missions are:
-- Insertion
-- Help for the elderly
-**Legal and voluntary aid**– Processing applications for health coverage and social assistance
-**– Domiciliation of people with no fixed or stable address**– Financial aid, emergency food aid, contribution to school canteen costs, transport aid, Christmas parcels…
-#### Address
-62 Rue de l'Évêché, 13002 Marseille
-#### Openings hours
--
-##### on working days (Mon - Fri)
-- 08:30 - 11:45
-- 12:45 - 16:30
-#### Contacts
--
-[Website](https://www.ccas-marseille.fr/vos-droits) -
-[+33491991460](tel:+33491991460)
-#### Suggest an edit
--
-[Write to QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Please, edit this place info&amp;body=CCAS (Community Social Action Center) – Center Agency (https://qx1.org/en/place/ccas-community-social-action-center-center-agency/) )</t>
-        </is>
-      </c>
-      <c r="B502" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_social_assistance_marseille", "info": "I need social assistance and guidance in Marseille, particularly if I am in a difficult situation such as homelessness, poverty, or disability."}, {"id": "need_legal_assistance_marseille", "info": "I need help with legal matters in Marseille."}, {"id": "need_housing_assistance_marseille", "info": "I need help with housing issues, such as finding housing or preventing eviction in Marseille."}, {"id": "need_domiciliation_marseille", "info": "I need a stable address (domiciliation) in Marseille."}], "Summary": {"country": "FR", "description": "The Community Social Action Center (CCAS) in Marseille, France provides various social services to individuals and families in need, including assistance with administrative procedures, financial aid, housing, and access to healthcare and social benefits.", "id": "ccas_center_agency_marseille", "type": "directory", "cities": ["Marseille"]}, "Contact": [{"id": "contact_ccas_marseille", "phone": "+33491991460", "contact_page": "https://www.ccas-marseille.fr/vos-droits", "city": "Marseille"}], "Organization": [{"id": "ccas", "info": "The CCAS (Community Social Action Center) in Marseille provides various social services to individuals and families in need.", "cities": ["Marseille"], "contacts": ["contact_ccas_marseille"]}], "Provision": [{"contexts": ["need_social_assistance_marseille"], "id": "social_assistance_and_support", "info": "Providing social assistance and support.", "organizations": ["ccas"]}, {"contexts": ["need_housing_assistance_marseille", "need_financial_assistance_marseille"], "id": "financial_assistance_and_housing_support", "info": "Providing financial aid, emergency food aid, contributions to school canteen costs, transport aid, and Christmas parcels.", "organizations": ["ccas"]}, {"contexts": ["need_legal_assistance_marseille"], "id": "legal_and_voluntary_aid", "info": "Offering legal and voluntary assistance, including processing applications for health coverage and social assistance.", "organizations": ["ccas"]}, {"contexts": ["need_domiciliation_marseille"], "id": "domiciliation_services", "info": "Providing domiciliation services for individuals with no fixed or stable address.", "organizations": ["ccas"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="503">
-      <c r="A503" t="inlineStr">
-        <is>
-          <t># Solidarité Provence Afghanistan (SPA)
-Fondée en Mars 2005, cette association a pour but de fournir une aide humanitaire aux populations d’Afghanistan, en particulier dans le domaine éducatif et d’organiser des rencontres culturelles et d’information sur l’Afghanistan.
-Adresse Postale :
-Solidarité Provence Afghanistan
-Cité des Associations
-Boîte aux lettres n° 29
-93 La Canebière, 13001 Marseille.
-Adresse mail : prov.afghanistan@wanadoo.fr
-#### Adresse
-Cité des Associations, 93 La Canebière, 13001 Marseille.
-#### Contacts
--
-[Site](https://solidarite-provence-afghanistan.com/) -
-[prov.afghanistan@wanadoo.fr](mailto:prov.afghanistan@wanadoo.fr)
-#### Proposer une modification
--
-[Écrire à QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Merci de modifier les infos de ce lieu&amp;body=Solidarité Provence Afghanistan (SPA) (https://qx1.org/lieu/solidarite-provence-afghanistan-spa/) )</t>
-        </is>
-      </c>
-      <c r="B503" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_support_for_afghanistan", "info": "I need information or support related to Afghanistan."}], "Summary": {"country": "FR", "description": "Solidarité Provence Afghanistan (SPA) is a non-profit organization in Marseille, France, dedicated to providing humanitarian aid to Afghanistan, particularly in the field of education, and organizing cultural events and information sessions about Afghanistan.", "id": "solidarite_provence_afghanistan_marseille", "type": "directory", "cities": ["Marseille"]}, "Contact": [{"id": "contact_solidarite_provence_afghanistan_marseille", "email": "prov.afghanistan@wanadoo.fr", "city": "Marseille"}], "Organization": [{"id": "solidarite_provence_afghanistan", "info": "Solidarité Provence Afghanistan (SPA) is an organization that provides humanitarian aid to Afghanistan.", "cities": ["Marseille"], "contacts": ["contact_solidarite_provence_afghanistan_marseille"], "website": "https://solidarite-provence-afghanistan.com/"}], "Provision": [{"contexts": ["need_support_for_afghanistan"], "id": "humanitarian_aid_afghanistan", "info": "Providing humanitarian aid, particularly in the field of education.", "organizations": ["solidarite_provence_afghanistan"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="504">
-      <c r="A504" t="inlineStr">
-        <is>
-          <t># Водительские права
-Статья опубликована 15/11/2023 • Последние изменения 14/08/2024
-Если в Париже еще можно обойтись без автомобиля, то в остальной Франции без машины никуда. В этой статье вы найдете подробный гайд по водительским правам во Франции: использование иностранных прав, процедура обмена, получение французских прав и основные правила дорожного движения
-[Самое важное, что нужно знать](https://exil-solidaire.fr#4a8f67ad6a1446f6851b9c5d9dbdbdc7)
-[Со скольких лет можно водить во Франции](https://exil-solidaire.fr#d9d7569f16904be8b8d6b00bdc1f6e1a)
-[Можно ли водить с иностранными правами?](https://exil-solidaire.fr#614013b86ce040fda63614b4e429216e)
-[Европейское водительское удостоверение](https://exil-solidaire.fr#bf87afb549604733968e492e1fa2745b)
-[Неевропейское водительское удостоверение](https://exil-solidaire.fr#884df9da8a1f465eb0152cf342295928)
-[Условия признания иностранного водительского удостоверения во Франции](https://exil-solidaire.fr#3f4902b4ad9040ccb5c6144b4007b564)
-[Штраф за использование иностранных прав после 1 года во Франции](https://exil-solidaire.fr#805f19117104402e895406aa5d20a4fa)
-[Как обменять водительское удостоверение](https://exil-solidaire.fr#037174b5998043a7924be2edc858e543)
-[Проверьте возможность обмена](https://exil-solidaire.fr#e29fd9b2f20b4d728083f818bbd0b741)
-[Какие категории прав можно обменять](https://exil-solidaire.fr#7a47c4d8c2e040c59f3ae30c40a661b0)
-[Условия для обмена](https://exil-solidaire.fr#978b7cd48937409a840c752614c567ca)
-[Сроки подачи](https://exil-solidaire.fr#bcbf52d8c81845c193ad202c20247576)
-[Процедура обмена](https://exil-solidaire.fr#8bfebf5bd52c4f7c9f8ed1c997705520)
-[Завершение процесса](https://exil-solidaire.fr#714beb199e994f539986dac0419278a3)
-[Особенности обмена прав для беженцев](https://exil-solidaire.fr#599073bd9e03464eb2acf2ef44681b35)
-[Как сдать на водительские права во Франции](https://exil-solidaire.fr#d13c3d543c5b4764a82495482cbf3cec)
-[Сколько стоит сдать на права во Франции?](https://exil-solidaire.fr#7a24c36afde24d3384f491ba4b3ce1e4)
-[Субсидии государства для получения водительских прав](https://exil-solidaire.fr#fa98e423ed284a4095df6a0e5f504b8e)
-[Какие документы нужны для получения водительских прав во Франции?](https://exil-solidaire.fr#64a0ebab99bb4bd4868077cd88b1a232)
-[Как выглядит водительское удостоверение во Франции](https://exil-solidaire.fr#91239fa87872481dbfcc7bba0094b5f9)
-[Основные правила дорожного движения](https://exil-solidaire.fr#d82c2742aeeb4d728a20b767069c88cc)
-[Балльная система водительских прав](https://exil-solidaire.fr#207e6b47509c4c878c40f01dd8c7a52f)
-[🔗 Полезные ссылки](https://exil-solidaire.fr#d4a793717ef940e09d4d4fe918599dd9)
-[❓FAQ](https://exil-solidaire.fr#30269d0cb8ac423b9528c4f235936e04)
-[Личный опыт авторов и читателей](https://exil-solidaire.fr#3c5beb176af0438cab9f841af63cad99)
-Самое важное, что нужно знать
-- Иностранные граждане, постоянно проживающие во Франции, могут водить с иностранными правами в течение одного года после начала действия их ВНЖ. И в течение этого года они должны успеть обменять свои права на французские или заново сдать на права.
-- Обмен прав возможен только для стран, с которыми у Франции есть двусторонние соглашение. Для остальных — необходимо заново сдавать на права. Россия входит в список стран, для которых обмен прав возможен. Для Украины и Беларуси необходимо заново сдавать на водительские права.
-- Просители международной защиты, обладатели APS, студенты, а также владельцы некоторых ВНЖ —
-*recherche d'emploi*/*création d'entreprise, jeune au pair, vacances-travail, retraité, stagiaire, travailleur saisonnier, travailleur temporaire*с ВНЖ, сроком менее 185 дней*—*могут пользоваться своими водительскими правами все время действия этих документов, проживание по этим документам не засчитывается в срок на обмен прав.
-- Бенифиары международной защиты имеют особые условия для обмена прав, включая возможность обмена просроченных прав и отсутствие необходимости предоставлять справку из страны происхождения.
-- Это правило не касается водительских прав, выданных в ЕС/ЕЭЗ — такими правами можно пользоваться без ограничений.
-- Французские права действуют 15 лет и работают по системе 12 баллов. При обмене прав, полученных менее 3 лет назад, — выдаются временные права с 6 баллами.
-- Процесс получения прав включает теоретический и практический экзамены. Стоимость обучения и экзаменов — от 1200 до 1800 евро.
-- Штрафы за вождение с недействительными иностранными правами могут достигать 15000 евро и включать лишение свободы до года.
-- Во Франции действуют строгие правила дорожного движения, включая ограничения скорости и допустимого уровня алкоголя в крови (0,5 г/л, для начинающих водителей — 0,2 г/л).
-Со скольких лет можно водить во Франции
-Всю информацию можно найти на
-[сайте](https://www.service-public.fr/particuliers/vosdroits/N530):
-Permis de conduire
-Permis de conduire : Attestation et brevet de sécurité routière, Permis moto, Permis B (voiture ou quadricycle lourd), Permis pour le transport de marchandises et de personnes, Perte, vol ou détérioration du permis de conduire, Contrôle médical
-https://www.service-public.fr/particuliers/vosdroits/N530
-Тип транспорта — категория | Разрешенный возраст |
-Легковые автомобили — B | с 18 лет можно получить полноценные водительские права
-с 15 лет можно начать обучение по системе «сопровождаемого вождения» (conduite accompagnée) |
-Мопеды до 50 куб. см — AM | с 14 лет, после прохождения специального обучения |
-Легкие мотоциклы до 125 куб. см — A1 | с 16 лет |
-Мотоциклы до 35 кВт — A2 | с 18 лет |
-Мотоциклы без ограничения мощности — A | с 20 лет, при наличии двухлетнего стажа вождения мотоцикла категории A2 |
-Грузовые автомобили — C | с 21 года |
-Автобусы — D | с 24 лет |
-Для некоторых категорий существуют дополнительные требования, такие как медицинские осмотры или профессиональная подготовка.
-Можно ли водить с иностранными правами?
-**Да, но есть нюансы:**
-Граждане ЕС/ЕЭЗ могут водить с национальными правами без ограничений.
-Гражданам других стран разрешено использовать иностранные права год после получения вида на жительство, затем потребуются французские права.
-Проверить, можно ли обменять ваши права можно
-[здесь](https://www.service-public.fr/simulateur/calcul/PermisEtrangerPermisFrancais):
-www.service-public.fr
-Vérifié le 12 Janvier 2023 - Direction de l'information légale et administrative (Premier ministre)
-https://www.service-public.fr/simulateur/calcul/PermisEtrangerPermisFrancais
-Европейское водительское удостоверение
-Если у вас есть водительское удостоверение, выданное государством-членом Европейского Союза (
-*Union Européenne*— UE) или[Европейскойэкономическойзоны](https://www.welcometofrance.com/fiche/espace-schengen)(*Espace Economique Européen*— EEE), такое «европейское» удостоверение является действительным на территории Франции**без ограничения срока действия**.**Страны Европейского Союза (ЕС):**
-Австрия, Бельгия, Болгария, Венгрия, Германия, Греция, Дания, Ирландия, Испания, Италия, Кипр, Латвия, Литва, Люксембург, Мальта, Нидерланды, Польша, Португалия, Румыния, Словакия, Словения, Финляндия, Франция, Хорватия, Чехия, Швеция, Эстония
-**Страны Европейской экономической зоны (ЕЭЗ):**
-Исландия, Лихтенштейн, Норвегия
-Швейцария (не член ЕС или ЕЭЗ, но участвует во многих соглашениях)
-Этот список актуален на август 2024 года. Состав ЕС и ЕЭЗ может меняться со временем.
-Неевропейское водительское удостоверение
-Если у вас есть водительское удостоверение, выданное вне ЕЭЗ, то оно действительно в течение первого года пребывания. То есть, иностранные водительские удостоверения действуют во Франции не более одного года с момента начала действия первого разрешения на пребывание во Франции, которым считается:
-- вид на жительство (
-*titre de séjour*) — с момента начала действия первого вида на жительство
-Читайте также:
-[ВНЖ | Вид на жительство](https://exil-solidaire.fr/titredesejour)
-- долгосрочная виза, эквивалентная виду на жительство (
-*visa de long séjour valant titre de séjour*— VLS-TS) — с момента валидации этой визы онлайн или в OFII
-Читайте также:
-[Visa D | Виза D | Долгосрочные визы](https://exil-solidaire.fr/visa-d)
-- подтверждение (
-*récépissé*) о получении международной защиты (OFPRA) — с момента вручения*récépissé*со статусом «признанный беженец», или «получивший дополнительную защиту», или «запросивший выдачу первого вида на жительство со статусом лица без гражданства» (API).
-Читайте также:
-[Типы международной защиты](https://exil-solidaire.fr/protection-internationale)
-[Решение по запросу убежища](https://exil-solidaire.fr/decision-ofpra)
-Срок в 1 год на обмен водительских прав не возобновляется, вне зависимости от изменения оснований для пребывания во Франции. Те, кто пропустил срок на обмен водительского удостоверения, должны будут заново сдавать на права во Франции в общем порядке.
-Просители международной защиты, обладатели APS, студенты, а также владельцы некоторых ВНЖ —
-*recherche d'emploi*/*création d'entreprise, jeune au pair, vacances-travail, retraité, stagiaire, travailleur saisonnier, travailleur temporaire*с ВНЖ*, сроком менее 185 дней —*могут пользоваться своими водительскими правами все время действия этих документов, проживание по этим документам не засчитывается в срок на обмен прав.Обмен
-**становится обязательным**, если водитель совершил нарушение, повлекшее за собой меры, такие как изъятие или приостановление прав.Условия признания иностранного водительского удостоверения во Франции
-Соблюдение этих условий обеспечит признание вашего водительского удостоверения во Франции.
-**Общие требования:**
-- обмен прав предусмотрен международным двухсторонним соглашением, которое исполняется на основе взаимности
-- удостоверение должно быть действующим
-- соблюдение медицинских ограничений (например, ношение очков)
-- достижение минимального возраста для вождения (18 лет для категории B)
-- действительность удостоверения в стране выдачи (без лишения прав или ограничений)
-**Дополнительные требования для неевропе</t>
-        </is>
-      </c>
-      <c r="B504" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_to_know_about_driving_in_france", "info": "I am a foreigner living in France and need information about driving licenses and road rules."}, {"id": "need_to_know_about_driving_with_foreign_license", "info": "I want to know if I can drive in France with my foreign driving license."}, {"id": "need_to_exchange_driving_license", "info": "I need to know how to exchange my foreign driving license for a French one."}, {"id": "need_to_take_driving_test_france", "info": "I need to take a driving test in France."}, {"id": "need_to_know_about_driving_rules_france", "info": "I need to learn about the main traffic rules in France."}, {"id": "need_to_know_about_driving_license_points_system", "info": "I need to understand the points system for driving licenses in France."}, {"id": "need_to_know_about_driving_license_for_refugees", "info": "I am a refugee and need information about exchanging driving licenses in France."}, {"id": "need_to_know_about_legalizing_irregular_status", "info": "I want to know about the possibility of legalizing my irregular status in France."}], "Summary": {"country": "FR", "description": "This guide provides comprehensive information about driving licenses in France, covering topics such as driving with foreign licenses, exchanging licenses, obtaining new licenses, and main traffic rules. It also includes information about the driving license points system, special considerations for refugees, and helpful links.", "id": "driving_license_guide_france", "type": "guide"}, "Organization": [{"id": "service_public_fr", "info": "Service Public is a website providing information on public services and procedures in France."}, {"id": "legifrance", "info": "Legifrance is a website providing access to French legal information."}, {"id": "prefecture", "info": "The Prefecture is the local government body that issues and manages residency permits."}, {"id": "ofii", "info": "The OFII (French Office for Immigration and Integration) manages administrative procedures for temporary residence permits."}, {"id": "welcometofrance", "info": "Welcome to France is a website providing information for foreigners arriving in France."}], "Provision": [{"contexts": ["need_to_know_about_driving_in_france", "need_to_know_about_driving_with_foreign_license", "need_to_exchange_driving_license", "need_to_know_about_driving_rules_france"], "id": "driving_license_information", "info": "Providing information on driving licenses and road rules in France.", "organizations": ["service_public_fr"]}, {"contexts": ["need_to_exchange_driving_license"], "id": "driving_license_exchange", "info": "Explaining the process of exchanging a foreign driving license for a French one.", "organizations": ["service_public_fr", "prefecture"]}, {"contexts": ["need_to_take_driving_test_france"], "id": "driving_test_information", "info": "Providing information on taking a driving test in France.", "organizations": ["service_public_fr"]}, {"contexts": ["need_to_know_about_driving_rules_france"], "id": "traffic_rules_information", "info": "Providing information about the main traffic rules in France.", "organizations": ["service_public_fr"]}, {"contexts": ["need_to_know_about_driving_license_points_system"], "id": "driving_license_points_system", "info": "Providing information about the driving license points system in France.", "organizations": ["service_public_fr"]}, {"contexts": ["need_to_know_about_driving_license_for_refugees"], "id": "refugee_driving_license_exchange", "info": "Providing information on special considerations for refugees regarding driving license exchange, including the possibility of exchanging expired licenses and not needing a certificate from the country of origin.", "organizations": ["service_public_fr", "prefecture", "ofii"]}, {"contexts": ["need_to_know_about_legalizing_irregular_status"], "id": "irregular_status_legalization", "info": "Providing information on the possibility of legalizing irregular status through exceptions to residency rules.", "organizations": ["prefecture"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="505">
-      <c r="A505" t="inlineStr">
-        <is>
-          <t># CS St.Gabriel Bon Secours support point
-Foreign nationals’ legal advice centre :
-- welcoming, informing and guiding foreign nationals or anyone facing a question related to foreigners’ rights (families, spouses of French nationals, etc.) in their administrative procedures related to living and working in France
-- build up administrative files, encouraging autonomy and responsibility
-- provide guidance and access to public services, without taking their place
-#### Address
-12 rue Richard 13014 MARSEILLE
-#### Contacts
--
-[pointdappui13014@gmail.com](mailto:pointdappui13014@gmail.com) -
-[+334 91 67 32 03](tel:+334 91 67 32 03)
-#### Suggest an edit
--
-[Write to QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Please, edit this place info&amp;body=CS St.Gabriel Bon Secours support point (https://qx1.org/en/place/cs-st-gabriel-bon-secours-support-point/) )</t>
-        </is>
-      </c>
-      <c r="B505" t="inlineStr">
-        <is>
-          <t>{"Contact": [{"id": "contact_cs_st_gabriel_marseille", "email": "pointdappui13014@gmail.com", "phone": "+334 91 67 32 03", "city": "Marseille"}], "Context": [{"id": "need_legal_advice_foreigners", "info": "I am a foreign national or have a question related to foreigners' rights and need assistance with administrative procedures in France."}], "Summary": {"country": "FR", "description": "CS St.Gabriel Bon Secours support point is a legal advice center in Marseille, France, offering support to foreign nationals with administrative procedures related to living and working in France.", "id": "cs_st_gabriel_bon_secours_marseille", "type": "directory", "cities": ["Marseille"]}, "Organization": [{"id": "cs_st_gabriel_bon_secours", "info": "CS St.Gabriel Bon Secours is a legal advice center that assists foreign nationals with administrative procedures.", "contacts": ["contact_cs_st_gabriel_marseille"], "cities": ["Marseille"]}], "Provision": [{"contexts": ["need_legal_advice_foreigners"], "id": "legal_advice_and_guidance", "info": "Providing legal advice and guidance to foreign nationals on administrative procedures related to living and working in France.", "organizations": ["cs_st_gabriel_bon_secours"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="506">
-      <c r="A506" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Être accompagné pour trouver un travail
-C'est quoi ?
-**C'est un dispositif de la Mission Locale qui aide les jeunes (entre 16 et 25 ans) à définir un projet professionnel et à trouver du travail. **Ce dispositif s'appelle le PACEA.
-Pour chaque jeune qui entre dans ce dispositif, la Mission Locale l'accompagne de manière personnalisée et l'aide à trouver un emploi. En fonction de la situation et des besoins, il est possible d'avoir une allocation financière (497€ maximum si le jeune ne reçoit pas d'autres aides).
-Pourquoi c'est intéressant ?
-Cet accompagnement permet au jeune d'avoir :
-- un référent unique
-- des rendez-vous individuels réguliers
-- la possibilité de participer à des ateliers collectifs
-- d'accéder à l'offre de service globale de la Mission Locale.
-En fonction de sa situation, le jeune peut bénéficier d'une allocation financière (sous condition).
-Comment faire ?
-Vous pouvez venir rencontrer un conseiller Mission Locale au siège **sans rendez-vous : **
-**64 Boulevard Léon Jouhaux à Clermont-Ferrand**
-- Les lundis, mercredis et jeudis de 8h30 à 11h30, et de 13h30 à 16h30
-- Les mercredis de 13h30 à 16h30
-- Les vendredis de 8h30 à 11h30
-Il est aussi possible de prendre rendez-vous pour rencontrer un conseiller sur une permanence extérieure.
-Pour cela, vous pouvez prendre rendez-vous par téléphone (**04.73.42.17.57)** ou en allant à l’accueil de la Mission Locale (64 Boulevard Léon Jouhaux à Clermont-Ferrand).
-## Addresses
-### Mission locale Clermont Métropole
-64 Bd Léon Jouhaux, 63100 Clermont-Ferrand, France
-</t>
-        </is>
-      </c>
-      <c r="B506" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_job_search_support", "info": "I need help finding a job in France."}, {"id": "need_career_guidance", "info": "I need help with career planning and guidance."}, {"id": "need_job_training_and_development", "info": "I need to learn new skills or get training for a job."}, {"id": "need_administrative_assistance", "info": "I need assistance with administrative procedures, such as obtaining health insurance or housing."}, {"id": "need_transportation_assistance", "info": "I need help with transportation and obtaining a driver's license."}, {"id": "need_financial_assistance_for_job_search", "info": "I need financial assistance to help with my job search efforts."}], "Summary": {"country": "FR", "description": "The Mission Locale in Clermont-Ferrand, France, provides support and guidance to help young people find jobs and integrate into the workforce. They offer personalized coaching, assistance with administrative tasks, and financial aid for job seekers.", "id": "mission_locale_clermont_ferrand", "type": "directory", "cities": ["Clermont-Ferrand"]}, "Contact": [{"id": "contact_mission_locale_clermont_clermont-ferrand", "phone": "04.73.42.17.57", "city": "Clermont-Ferrand", "address": "64 Bd Léon Jouhaux, 63100 Clermont-Ferrand, France"}], "Organization": [{"id": "mission_locale_clermont_metropole", "info": "The Mission Locale in Clermont-Ferrand is an organization that provides support services to young people in their job search and career development.", "cities": ["Clermont-Ferrand"], "contacts": ["contact_mission_locale_clermont_clermont-ferrand"]}], "Provision": [{"contexts": ["need_job_search_support", "need_career_guidance", "need_job_training_and_development", "need_administrative_assistance", "need_transportation_assistance"], "id": "job_search_and_integration_support", "info": "Providing support and guidance to help job seekers with their career development, administrative tasks, and finding job opportunities.", "organizations": ["mission_locale_clermont_metropole"]}, {"contexts": ["need_financial_assistance_for_job_search"], "id": "financial_assistance", "info": "Offering financial assistance to help with job search.", "organizations": ["mission_locale_clermont_metropole"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="507">
-      <c r="A507" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Reçus à la Plateforme au troisième essai
-Une famille soudanaise qu’on connaissait de l’Italie […] nous a expliqué comment faire pour demander l’asile et nous a dit qu’on devait aller à la Plateforme. On y est allés mais on est arrivés trop tard, à 8h30 il n’y a déjà plus de place pour les nouveaux arrivants. […] Alors on est retourné deux jours plus tard, à 6h00 du matin mais on n’a pas pu s’inscrire sur la liste géré par l’agent de sécurité à l’ouverture… on a pas pu entrer. Finalement trois jours après on a réussi. Ils nous ont donné le rendez vous pour la Préfecture pour la mi-octobre 2017, une longue attente…
-La famille doit attendre 51 jours d’attente pour pouvoir déposer sa demande d’asile. Quand nous les rencontrons ils sont dans cette attente.
-[PADA](https://qx1.org/lieu/pada-marseille/)
-Les PADA sont la porte d’entrée dans la procédure d’asile : toute personne qui souhaite demander l’asile doit s’y présenter pour obtenir une convocation au Guichet unique pour demandeur d’asile (GUDA)
-</t>
-        </is>
-      </c>
-      <c r="B507" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "asylum_application_process_marseille", "info": "I need to apply for asylum in Marseille, France."}, {"id": "need_assistance_with_asylum_application", "info": "I need assistance in navigating the asylum process."}, {"id": "need_to_schedule_guda_appointment", "info": "I need to schedule an appointment for asylum application registration at the GUDA."}], "Summary": {"country": "FR", "description": "This text recounts a family's experience with the Plateforme Asile in Marseille, France, highlighting the long wait times and challenges they faced while trying to register their asylum application. The experience underscores the difficulties and bureaucracy asylum seekers often encounter.", "id": "plateforme_asile_marseille_experience", "type": "experience", "cities": ["Marseille"]}, "Organization": [{"id": "pada", "info": "PADA (Premier Accueil des Demandeurs d'Asile) are the first reception centers for asylum seekers, where they receive information and are scheduled for GUDA appointments.", "cities": ["Marseille"]}, {"id": "plateforme_asile", "info": "Plateforme Asile is an organization that provides assistance to asylum seekers in Marseille.", "cities": ["Marseille"], "provisions": ["asylum_application_registration_support"]}], "Provision": [{"contexts": ["asylum_application_process_marseille", "need_assistance_with_asylum_application"], "id": "asylum_application_registration", "info": "Registering asylum applications.", "organizations": ["pada"]}, {"contexts": ["need_to_schedule_guda_appointment"], "id": "schedule_guda_appointment", "info": "Scheduling appointments for asylum application registration.", "organizations": ["pada"]}, {"contexts": ["asylum_application_process_marseille", "need_assistance_with_asylum_application"], "id": "asylum_application_registration_support", "info": "Providing assistance with asylum application registration.", "organizations": ["plateforme_asile"]}], "Task": [{"contexts": ["asylum_application_process_marseille"], "id": "go_to_plateforme_asile", "info": "Going to the Plateforme Asile for asylum application assistance.", "provisions": ["asylum_application_registration_support"]}, {"contexts": ["need_to_schedule_guda_appointment"], "id": "request_guda_appointment", "info": "Requesting a GUDA appointment.", "provisions": ["schedule_guda_appointment"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="508">
-      <c r="A508" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Des conditions difficiles à l’UHU Madrague
-Un africain croisé à la gare m’a dit que je pouvais appeler le 115 le 3éme jour. Ils sont venus me chercher et m’ont emmené à la UHU Madrague où je suis resté 4 mois. C’était pas bien là bas.
-De 7 heures du matin il faut sortir. Il faisait très froid. Je passais les journées dehors sans savoir où aller, sans avoir à manger. Avec ma blessure c’était très dur parce que j’ai une plaie ouverte au pied et le froid rentre. J’allais à l’accueil de jour mais là bas il ne donne pas à manger.
-J’ai décidé de quitter l’UHU Madrague en août parce que c’était la guerre là bas, les gens se battaient avec des couteaux. Quand tu dors un fou vient te frapper, les portes des chambres sont toujours ouvertes et tout le monde entre. On est 6 dans les chambres et il y a tout le monde (toute sorte de personnes).
-Je ne pouvais plus supporter cette ambiance tendue et je suis parti. J’ai rappelé le 115 et ils m’ont donné 9 nuits à Forbin. Plus tard, j’ai rappelé et ils ont renouvelés une fois pour 9 nuits supplémentaires puis ils ont arrêté en disant que il n’y avait plus de place.
-</t>
-        </is>
-      </c>
-      <c r="B508" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "homeless_in_marseille", "info": "I am experiencing homelessness in Marseille, France."}, {"id": "staying_at_uhu_madrague", "info": "I am staying at the UHU Madrague emergency shelter in Marseille."}, {"id": "difficulty_accessing_services_uhu_madrague", "info": "I am struggling to access basic services and support at the UHU Madrague, such as food and healthcare."}, {"id": "uncomfortable_environment_uhu_madrague", "info": "The environment at the UHU Madrague is unsafe and uncomfortable, with violence and lack of security."}, {"id": "need_alternative_accommodation_marseille", "info": "I need to find alternative accommodation in Marseille due to the conditions at the UHU Madrague."}, {"id": "need_assistance_115", "info": "I need to contact the 115 emergency hotline for help with finding accommodation."}], "Summary": {"country": "FR", "description": "A personal account of a migrant's experience staying at the UHU Madrague emergency shelter in Marseille, France, highlighting the difficult conditions and lack of access to essential services, leading to their eventual departure and reliance on the 115 hotline for alternative accommodation.", "id": "uhu_madrague_experience", "type": "experience", "cities": ["Marseille"]}, "Organization": [{"id": "uhu_madrague", "info": "UHU Madrague is an emergency shelter in Marseille.", "cities": ["Marseille"]}, {"id": "115_marseille", "info": "The 115 emergency hotline in Marseille.", "cities": ["Marseille"]}, {"id": "forbin_shelter", "info": "Forbin is another emergency shelter in Marseille.", "cities": ["Marseille"]}], "Provision": [{"contexts": ["homeless_in_marseille", "need_assistance_115"], "id": "emergency_accommodation_115", "info": "Providing emergency accommodation services to homeless individuals.", "organizations": ["115_marseille"]}, {"contexts": ["staying_at_uhu_madrague", "difficulty_accessing_services_uhu_madrague", "uncomfortable_environment_uhu_madrague", "need_alternative_accommodation_marseille"], "id": "uhu_madrague_services", "info": "Providing emergency shelter and basic services for homeless individuals.", "organizations": ["uhu_madrague"]}, {"contexts": ["need_alternative_accommodation_marseille"], "id": "forbin_shelter_services", "info": "Providing emergency shelter services.", "organizations": ["forbin_shelter"]}], "Task": [{"contexts": ["homeless_in_marseille", "need_assistance_115"], "id": "contact_115", "info": "Contacting the 115 emergency hotline for accommodation.", "contacts": "115_marseille", "provisions": ["emergency_accommodation_115"]}, {"contexts": ["need_alternative_accommodation_marseille"], "id": "contact_115_for_alternative_accommodation", "info": "Contacting the 115 emergency hotline for alternative accommodation.", "contacts": "115_marseille", "provisions": ["emergency_accommodation_115"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="509">
-      <c r="A509" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Faire un chantier d'insertion en restauration
-C'est quoi ?
-Le chantier d’insertion Brasserie l’Encas prépare des repas destinés aux personnes qui fréquentent l’École des Métiers (apprentis et personnels) et aux particuliers, du lundi au vendredi avec deux services, 12h et 13h.
-Pourquoi c'est intéressant ?
-En participant à ce chantier d'insertion, vous serez salarié du chantier.
-Vous serez accompagné pendant tout votre chantier d'insertion, avec un suivi individuel.
-Une formation de français est proposée sur le temps de travail à l’École des Métiers.
-Un chantier d’insertion a pour but d'aider des personnes en difficulté à trouver un emploi ou une formation.
-Comment faire ?
-Demandez à votre conseiller de contacter les chantiers d'insertion de l’École des Métiers.
-- Mail : contact@ecoledesmetiers.fr
-- Tel : 0380684880
-## Addresses
-### Ecole des Métiers Dijon Métropole - EDM
-1 Chem. de la Noue, 21600 Longvic, France
-</t>
-        </is>
-      </c>
-      <c r="B509" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_to_access_work_integration_program", "info": "I need to find a work integration program in France."}, {"id": "need_french_language_training_for_work", "info": "I need French language training tailored for the workplace."}], "Summary": {"country": "FR", "description": "This guide explains a work integration program called Brasserie l'Encas in Dijon, France.  The program provides paid work experience in a restaurant, French language training, and support services to help individuals find employment or further training.", "id": "brasserie_lencas_work_integration_dijon", "type": "guide", "cities": ["Dijon"]}, "Contact": [{"id": "contact_ecoledesmetiers_email_dijon", "email": "contact@ecoledesmetiers.fr", "city": "Dijon"}, {"id": "contact_ecoledesmetiers_longvic", "address": "1 Chem. de la Noue, 21600 Longvic, France", "city": "Longvic", "phone": "0380684880", "email": "contact@ecoledesmetiers.fr"}, {"id": "contact_ecoledesmetiers_email_dijon", "city": "Dijon", "phone": "0380684880", "email": "contact@ecoledesmetiers.fr"}], "Organization": [{"id": "ecoledesmetiers", "info": "Ecole des Métiers is an organization that offers various training programs, including work integration programs.", "cities": ["Dijon", "Longvic"], "contacts": ["contact_ecoledesmetiers_email_dijon"]}], "Provision": [{"contexts": ["need_to_access_work_integration_program"], "id": "work_integration_program", "info": "Providing paid work experience in a restaurant setting.", "organizations": ["ecoledesmetiers"]}, {"contexts": ["need_french_language_training_for_work"], "id": "french_language_training_for_work", "info": "Offering French language training for the workplace.", "organizations": ["ecoledesmetiers"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="510">
-      <c r="A510" t="inlineStr">
-        <is>
-          <t># أخوية لا بيل دو مي (La Fraternité de la Belle de Mai)
-- ولوج مفتوح للمعلوميات وتكوين ذاتي بـ 5 أورو/السنة: وورد، إكسيل، أنترنت، مراسلات، الولوج للحقوق، الإجراءات الإدارية.
-- كاتب عمومي ( رسائل شخصية، سير ذاتية، طلبات البحث عن الشغل) (بالمــجــان).
-- وجبة الأخوية ب3 أورو للوجبة.
-- أنشطة ثقافية وأخوية (فسيفساء، بستنة، جولات وخرجات) : اطلبوا معلومات إضافية في عين المكان.
-- ورشة تعلم الفرنسية : اطلبوا معلومات إضافية في عين المكان، 5 أورو للسنة.
-- سوق مفتوح.
-**مغلق صيف 2024: من 1 إلى 31 غشت.**
-#### عناوين
-7, boulevard Burel, 13003 Marseille
-#### توقيت الفتح
--
-##### استقبال عام.
-##### يومياً
-- طيلة اليوم
-##### وجبة بثمن زهيد (3 أورو).
-##### ثٌلَاثَاءْ
-- 12:30 - 13:30
-##### الخميس
-- 12:30 - 13:30
-##### ورشة معلوميات.
-##### الاثنين
-- 14:00 - 16:45
-##### ثٌلَاثَاءْ
-- 09:00 - 12:00
-- 14:00 - 16:45
-##### الخميس
-- 09:00 - 12:00
-- 18:30 - 20:30
-##### كاتب العمومي
-##### الاثنين
-- 09:00 - 11:30
-- 14:00 - 16:30
-##### الخميس
-- 09:00 - 11:30
-- 14:00 - 16:30
-##### ورشات لتعلم الفرنسية - باستثناء يوم الأربعاء.
-##### on working days (Mon - Fri)
-- 10:00 - 12:00
-##### ورشة قراءة - كتابة.
-##### الخميس
-- 14:00 - 16:00
-##### سوق حر للملابس (باستثناء العطل المدرسية).
-##### ثٌلَاثَاءْ
-- 09:00 - 12:00
-##### الخميس
-- 09:00 - 12:00
-##### دروس للغة الفرنسية (من طرف جمعية آفيڤ AFEV.
-##### الاثنين
-- 13:30 - 15:30
-##### سوق حر للملابس المجانية بتوجيه من شريك لنا.
-##### الاثنين
-- 09:00 - 12:00
-##### مداومة ثقافية.
-##### ثٌلَاثَاءْ
-- 11:00 - 15:00
-##### ورشة بستنة Rinté.
-##### الخميس
-- 14:00 - 17:00
-##### ورشة رياضة خفيفة Gym Douce للــنــســاء.
-##### الاثنين
-- 09:00 - 11:00
-##### ورشة رياضة للعجزة.
-##### ثٌلَاثَاءْ
-- 14:00 - 16:45
-##### الخميس
-- 14:00 - 16:45
-#### للتواصل
--
-[موقع](http://labelledemai1.free.fr/?fbclid=IwAR1k2Nn0ciXSbhcDE_b7gHE8YJ0LwxGEk0TdlZQuQxg9E9A8FCBMNHwyV6I) -
-[labelledemai1@free.fr](mailto:labelledemai1@free.fr) -
-[+33491622809](tel:+33491622809)
-#### اقترح تعديل
--
-[أكتب ل Qx1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Please, edit this place info&amp;body=أخوية لا بيل دو مي (La Fraternité de la Belle de Mai) (https://qx1.org/ar/place/%d8%a3%d8%ae%d9%88%d9%8a%d8%a9-%d9%84%d8%a7-%d8%a8%d9%8a%d9%84-%d8%af%d9%88-%d9%85%d9%8a-la-fraternite-de-la-belle-de-mai/) )</t>
-        </is>
-      </c>
-      <c r="B510" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_computer_access", "info": "I need access to computers and internet."}, {"id": "need_administrative_support", "info": "I need help with administrative procedures and paperwork."}, {"id": "need_french_language_classes", "info": "I need to learn French."}, {"id": "need_affordable_meal", "info": "I need a cheap and affordable meal."}, {"id": "need_cultural_activities", "info": "I am looking for cultural activities and events."}, {"id": "need_second_hand_clothing", "info": "I need to find second-hand clothes."}, {"id": "need_garderie_services", "info": "I need childcare services for my children."}, {"id": "need_safe_space_for_women", "info": "I am a woman looking for a safe and welcoming space."}, {"id": "need_sexual_health_info", "info": "I need information on sexual health, contraception, or abortion."}, {"id": "need_housing_support", "info": "I need help finding housing."}, {"id": "need_support_for_prostitution", "info": "I need support for a situation involving prostitution."}, {"id": "need_clothing_repair", "info": "I need to repair my clothes."}, {"id": "need_free_wifi", "info": "I need free wifi."}, {"id": "need_healthcare_services", "info": "I need access to healthcare services."}], "Summary": {"country": "FR", "description": "La Fraternité de la Belle de Mai is a community center in Marseille, France, offering a wide range of support services including computer access, administrative assistance, French language classes, affordable meals, cultural activities, and more.", "id": "fraternite_belle_de_mai_marseille", "type": "directory", "cities": ["Marseille"]}, "Contact": [{"id": "contact_labelledemai_marseille", "email": "labelledemai1@free.fr", "phone": "+33491622809", "city": "Marseille"}], "Organization": [{"id": "labelledemai", "info": "La Fraternité de la Belle de Mai is a community center offering a wide range of services and activities for residents of the Belle de Mai neighborhood.", "cities": ["Marseille"], "contacts": ["contact_labelledemai_marseille"], "website": "http://labelledemai1.free.fr/?fbclid=IwAR1k2Nn0ciXSbhcDE_b7gHE8YJ0LwxGEk0TdlZQuQxg9E9A8FCBMNHwyV6I"}, {"id": "afev", "info": "AFEV is an association that provides French language classes.", "cities": ["Marseille"]}], "Provision": [{"contexts": ["need_computer_access", "need_administrative_support"], "id": "computer_access_and_administrative_support", "info": "Providing computer access, internet, and administrative assistance.", "organizations": ["labelledemai"]}, {"contexts": ["need_administrative_support"], "id": "legal_assistance", "info": "Offering legal assistance and document preparation services.", "organizations": ["labelledemai"]}, {"contexts": ["need_affordable_meal"], "id": "affordable_meal", "info": "Providing affordable meals.", "organizations": ["labelledemai"]}, {"contexts": ["need_cultural_activities"], "id": "cultural_activities_and_workshops", "info": "Offering cultural activities and workshops.", "organizations": ["labelledemai"]}, {"contexts": ["need_french_language_classes"], "id": "french_language_classes", "info": "Providing French language classes.", "organizations": ["labelledemai", "afev"]}, {"contexts": ["need_second_hand_clothing"], "id": "free_clothing_distribution", "info": "Organizing free clothing distribution events.", "organizations": ["labelledemai"]}, {"contexts": ["need_garderie_services"], "id": "childcare", "info": "Providing childcare services.", "organizations": ["labelledemai"]}, {"contexts": ["need_safe_space_for_women"], "id": "safe_space_for_women", "info": "Providing a safe and welcoming space for women.", "organizations": ["labelledemai"]}, {"contexts": ["need_sexual_health_info"], "id": "sexual_health_support", "info": "Providing confidential consultations on sexual health, contraception, and abortion.", "organizations": ["planning_familial"]}, {"contexts": ["need_housing_support"], "id": "housing_assistance", "info": "Offering housing assistance and support.", "organizations": ["labelledemai", "ampil"]}, {"contexts": ["need_support_for_prostitution"], "id": "prostitution_support", "info": "Providing support services for people involved in prostitution.", "organizations": ["amicale_du_nid"]}, {"contexts": ["need_clothing_repair"], "id": "clothing_repair_workshop", "info": "Offering a workshop for repairing clothing.", "organizations": ["atelier_textile_marhaban"]}, {"contexts": ["need_free_wifi"], "id": "free_wifi_access", "info": "Providing free wifi access.", "organizations": ["manifesten"]}, {"contexts": ["need_healthcare_services"], "id": "healthcare_services", "info": "Providing healthcare access and information.", "organizations": ["comede", "planning_familial", "pass_conception_maternite", "pass_mere_enfant", "mds"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="511">
-      <c r="A511" t="inlineStr">
-        <is>
-          <t># OFPRA (French Office for the Protection of Refugees and Stateless Persons)
-**Ofpra is a public administrative body created by the law of 25 July 1952.** It is responsible for applying the Geneva Convention relating to the Status of Refugees of 28 July 1951, and subsequently the New York Convention of 1954, and makes independent decisions on asylum and statelessness applications submitted to it.
-Ofpra has **three main missions**:
-**Examining applications**for international protection on the basis of the Geneva Convention of 28 July 1951, the New York Convention of 28 September 1954 and the CESEDA.**Legal and administrative protection**for statutory refugees, statutory stateless persons and beneficiaries of subsidiary protection.- Ofpra also advises on asylum procedures at the border. It issues
-**an opinion to the Minister of the Interior**on whether or not an application for authorisation to enter French territory on asylum grounds is manifestly well-founded.
-Address (in Paris):
-Rue Carnot 201, 94120 Fontenay-sous-Bois, Île-de-France France
-#### Address
-201 Rue Carnot, 94136 Fontenay-sous-Bois
-#### Suggest an edit
--
-[Write to QX1 (contact@qx1.org)](mailto:contact@qx1.org?subject=Please, edit this place info&amp;body=OFPRA (French Office for the Protection of Refugees and Stateless Persons) (https://qx1.org/en/place/ofpra-french-office-for-the-protection-of-refugees-and-stateless-persons/) )</t>
-        </is>
-      </c>
-      <c r="B511" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_to_apply_for_asylum", "info": "I need to apply for asylum in France."}, {"id": "need_to_know_about_ofpra", "info": "I need information on how to apply for asylum and the role of OFPRA."}, {"id": "need_to_learn_about_refugee_rights", "info": "I need to know about my rights as a refugee or beneficiary of international protection."}], "Summary": {"country": "FR", "description": "OFPRA (Office français de protection des réfugiés et apatrides) is a public administrative body in France responsible for examining asylum and statelessness applications.", "id": "ofpra_description", "type": "guide"}, "Organization": [{"id": "ofpra", "info": "OFPRA is a public administrative body responsible for examining asylum and statelessness applications."}], "Provision": [{"contexts": ["need_to_apply_for_asylum", "need_to_know_about_ofpra"], "id": "asylum_application_processing", "info": "Examining asylum and statelessness applications.", "organizations": ["ofpra"]}, {"contexts": ["need_to_learn_about_refugee_rights"], "id": "refugee_rights_information", "info": "Providing legal and administrative protection for refugees, stateless persons, and beneficiaries of subsidiary protection.", "organizations": ["ofpra"]}]}</t>
-        </is>
-      </c>
-    </row>
-    <row r="512">
-      <c r="A512" t="inlineStr">
-        <is>
-          <t># Несанкционированный въезд
-Статья опубликована 13/11/2023
-Будьте осторожны: при незаконном въезде (entrée irrégulière) на территорию Франции вы подвергаете себя существенным рискам, в том числе вы рискуете оказаться в критичной административной ситуации на длительный срок. В этой статье мы дадим определение незаконному въезду (entrée irrégulière). Легализация нелегального положения (regularisation) будет рассмотрена в другой статье, посвященной нелегальному пребыванию (sejour irrégulier).
-[Самое важное, что нужно знать](https://exil-solidaire.fr#ddc50641c6fe43e0a17bcfa55f939324)
-[Исключение ответственности (exceptions dépénalisantes)](https://exil-solidaire.fr#42f0e5a2adce4671b25f6c3e1af2dd05)
-[Содействие в нелегальном въезде и пребывании (соучастие)](https://exil-solidaire.fr#db912b95f67b483d81939a0c0893c29d)
-[Запреты на въезд (IRTF) и шенгенские предупреждения](https://exil-solidaire.fr#f7cbf2eeb92a47bd8260bbbbd5c19bd7)
-[🔗 Полезные ссылки](https://exil-solidaire.fr#91369e208b594267a3ecb2d60f56d401)
-[❓FAQ](https://exil-solidaire.fr#35b92c3e97d440e0b8c1ac4640d5d074)
-[Личный опыт авторов и читателей](https://exil-solidaire.fr#9797e662ab7b4dbaaa843cd2158f40d1)
-Самое важное, что нужно знать
-**Незаконный въезд**во Францию означает ситуацию, когда иностранец въезжает на территорию страны не имея необходимых документов (в частности, визы).
-**Незаконный въезд во Францию является преступлением средней тяжести (délit)**: преступление считается совершенным, если иностранец без должных документов задержан «на месте преступления», то есть в момент пересечения границы. Уголовное наказание, которому может быть подвергнут иностранец, может заключаться в тюремном заключении сроком на один год и штрафе в размере 3 750 евро. Также по решению уголовного суда нарушителю грозит дальнейший запрет на въезд на территорию Франции.
-Кроме того, незаконный въезд исключает возможность подачи заявления на получение вида на жительство вне процедуры регуляризации. Нелегала могут арестовать в момент подачи документов на получение вида на жительство с последующей процедурой выдворения из страны.
-Таким образом, нелегальный въезд автоматически влечёт за собой статус нелегального мигранта, проживающего в неурегулированной ситуации (sejour irrégulier).
-Напротив,
-**нелегальное пребывание****(maintien irrégulier)**во Франции означает ситуацию, когда иностранец законно въехал на государственную территорию, но не покинул её даже когда срок действия его вида на жительство истёк и/или его запрос на продление вида на жительство был отклонен (или ему было отказано в предоставлении статуса получателя международной защиты и он не выполнил обязательство покинуть территорию Франции в течение одного месяца).Читайте также:
-[Нелегальное пребывание и регуляризация](https://exil-solidaire.fr/sejour-irregulier)
-Для того чтобы пребывание иностранца в стране стало нелегальным (maintien irrégulier), такая ситуация должна продолжаться более трёх месяцев.
-**В первом и втором случае (незаконный въезд или нелегальное пребывание) иностранец находится в нелегальном положении (situation irrégulière), поскольку у него нет документа, позволяющий въезд или пребывание на территории.**
-В просторечии его называют «нелегальным иммигрантом» («sans-papier») или «нелегалом» («clandestin»).
-Исключение ответственности (exceptions dépénalisantes)
-Если принимающее государство не дало официального разрешения на въезд, то присутствие гражданина третьей страны может считаться данным государством незаконным. Вместе с тем, и в законодательстве ЕС, и в Европейской конвенции по правам человека указаны обстоятельства, при которых присутствие гражданина третьей страны должно считаться законным, даже если оно не санкционировано:
-- Лица, ищущие международную защиту
-- Жертвы торговли людьми и особо эксплуататорских условий труда на территории ЕС
-Читайте также:
-Содействие в нелегальном въезде и пребывании (соучастие)
-Во Франции въезд, пребывание и передвижение иностранцев с нелегальным статусом преследуется по закону. Аналогично помощь, оказываемая нелегальным мигрантам, является уголовным преступлением в соответствии с законодательным декретом от
-**2 мая 1938 года**об иммиграционной полиции (сегодня[статьяL.622-1](https://www.legifrance.gouv.fr/codes/id/LEGISCTA000006147789/2005-03-01)CESEDA). Однако с 1996 года были прописаны случаи освобождения от уголовного преследования.Статья L. 622-1 CESEDA, изначально направленная на борьбу с подпольными сетями контрабандистов и торговлей людьми, также может быть применена против частных лиц и ассоциаций, помогающих нелегальным мигрантам. Законодательство постепенно ввело некоторые послабления для некоторых групп лиц с целью
-**освобождения их от уголовного преследования**.[Законот22июля1996года,направленныйнаборьбустерроризмом](https://www.legifrance.gouv.fr/loda/id/JORFTEXT000000367689), учредил
-**«семейный иммунитет»**в пользу супруга/супруги иностранца, а также его родственников по восходящей и нисходящей линиям.
-[Законот11мая1998года,известныйкак«ЗаконRESEDA»](https://www.legifrance.gouv.fr/loda/id/JORFTEXT000000191302), расширил этот «иммунитет» на супругов вышеуказанных родственников, а также на братьев и сестёр мигранта и его/её супруги /супруга.
-Впоследствии
-[законот26ноября2003г.,касающийсяконтроляиммиграции,пребыванияиностранцеввоФранцииигражданства](https://www.legifrance.gouv.fr/loda/id/JORFTEXT000000795635), ужесточил наказание за соучастие в нелегальной иммиграции. Одновременно он обозначил рамки**«гуманитарного иммунитета»,**направленного на освобождение от уголовного преследования тех, кто оказывает помощь мигрантам, чьей жизни или физической неприкосновенности угрожает*«сиюминутная или неминуемая опасность»*.Общественные дебаты достигли своего апогея когда Седрик Эрру, фермер-активист из Приморских Альп, был арестован четыре раза в период с 2016 по 2017 год за содействие въезду во Францию и передвижению нелегальных мигрантов. В 2017 году он был приговорен к четырём месяцам тюремного заключения с отсрочкой за то, что помог примерно 200 нелегальным мигрантам пересечь итальянскую границу. В 2021 году Кассационный суд на основании решения Конституционного суда окончательно оправдал Седрика Эрру. Вследствие этого дела «гуманитарный иммунитет» был в очередной раз подтвержден
-**законом от 10 сентября 2018 года**.- Исключения распространяются на содействие как нелегальному пребыванию, так и нелегальному передвижению;
-- Так называемые «гуманитарные» исключения, предусмотренные в статье L. 622-4, 3°, применяются к физическому или юридическому лицу при следующих условиях:
-1° Инкриминированное действие не связано с какой-либо прямой или косвенной компенсацией.
-2° Оно (действие) представляло собой:
-- Практические советы/ консультации или юридическое, языковое, социальное сопровождение,
-- любая другая помощь, оказанная исключительно из гуманитарных соображений.
-Запреты на въезд (IRTF) и шенгенские предупреждения
-В связи с обязательством покинуть Францию (obligation de quitter la France - OQTF) префект полиции может принять решение о запрете последующего въезда на территорию Франции (interdiction de retour sur le territoire français - IRTF). Решение префекта возможно оспорить через подачу обращения (recours). Суд может признать запрет несостоятельным (annulée) и отменить его (abrogée)
-*.*Иностранец, не соблюдающий запрет на въезд, рискует подвергнуться уголовному преследованию.Запрет на въезд означает, что лицам запрещается въезжать в государство, из которого они высланы. Запрет обычно действует в течение определенного периода времени и обеспечивает, чтобы лицам, считающимся опасными или нежелательными, не выдавали визы или иным образом не допускали на территорию государства.
-В отношении лиц, подпадающих под запрет на въезд, вынесенный в связи
-с Директивой о возвращении незаконных мигрантов (
-[Директива2008/115/EC](https://eur-lex.europa.eu/legal-content/FR/TXT/HTML/?uri=CELEX:32008L0115)), такой запрет обычно действует не более пяти лет. Он обычно сопровождается предупреждением ШИС, и таким лицам запрещается доступ на всю территорию Шенгенской зоны. Для того чтобы другое государство-член ЕС могло выдать визу такому лицу или допустить его на свою территорию, государство-член ЕС, наложившее запрет на въезд, должно будет аннулировать этот запрет. Поскольку запрет мог быть обусловлен ситуацией, специфической для конкретного государства, наложившего такой запрет, то возникают вопросы о соразмерности санкций, особенно в случаях, касающихся других основных прав, например, при воссоединении семьи.Запреты на въезд, наложение которых не связано с выполнением Директивы о возвращении, формально не возбраняют другим государствам позволять въезд в Шенгенскую зону. Тем не менее другие государства могут учитывать запреты на въезд при принятии решений о том, выдавать ли визу или разрешать ли въезд. Поэтому запреты могут действовать на всей территории Шенгенской зоны, даже при том, что запрет может быть актуальным только для наложившего его государства, которое считает данное лицо нежелательным.
-Если вы вернетесь во Францию во время действия IRTF (interdiction de retour sur le territoire français), уголовный суд может приговорить вас к тюремному заключению на срок до 3 лет. А также вы можете подпасть под временный или бессрочный запрет пребывания на территории Франции (
-[interdictionduterritoirefrançais-ITF)](https://www.service-public.fr/particuliers/vosdroits/F2784).🔗 Полезные ссылки
-- Legifrance
-Chapitre Ier : Entrée irrégulière (Article L621-2) - Légifrance
-Code de l'entrée et du séjour des étrangers et du droit d'asile &gt; Chapitre Ier : Entrée irrégulière (Article L621-2)
-https://www.legifrance.gouv.fr/codes/section_lc/LEGITEXT000006070158/LEGISCTA000006147788/
-❓FAQ
-**Есть ли способы узаконить своё положение?**
-Легализация лиц, незаконно проживающих на территории Франции (sans papier), возможна.
-**Эта процедура позволяет обратиться к префекту с просьбой об исключительном разрешении остаться в стране (admission exceptionnelle au séjour). Префект в</t>
-        </is>
-      </c>
-      <c r="B512" t="inlineStr">
-        <is>
-          <t>{"Context": [{"id": "need_to_know_about_helping_irregular_migrants", "info": "I want to understand the legal risks involved in assisting irregular migrants in France, and whether there are exceptions."}, {"id": "need_to_know_about_entry_bans", "info": "I need information about entry bans and Schengen warnings."}, {"id": "need_to_know_about_legalizing_irregular_status", "info": "I want to know about the possibility of legalizing my irregular status in France."}], "Summary": {"country": "FR", "description": "This article defines illegal entry (entrée irrégulière) and irregular stay (séjour irrégulier) in France. It explains the legal consequences of these situations, including potential penalties and consequences for accessing residency rights. The article also discusses exceptions and legal frameworks for assistance to irregular migrants and entry bans.", "id": "illegal_entry_and_stay_france", "type": "guide"}, "Provision": [{"contexts": ["need_to_know_about_helping_irregular_migrants"], "id": "assistance_to_irregular_migrants", "info": "Providing information on exceptions and legal frameworks for assisting irregular migrants.", "organizations": ["legifrance"]}, {"contexts": ["need_to_know_about_legalizing_irregular_status"], "id": "irregular_status_legalization", "info": "Providing information on the possibility of legalizing irregular status through exceptions to residency rules.", "organizations": ["prefecture"]}, {"contexts": ["need_to_know_about_entry_bans"], "id": "entry_ban_information", "info": "Providing information on entry bans (IRTF) and Schengen warnings.", "organizations": ["legifrance"]}]}</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>